<commit_message>
Made necessary changes so everything works together.
</commit_message>
<xml_diff>
--- a/Xls/data.xlsx
+++ b/Xls/data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>slno</t>
   </si>
@@ -21,112 +21,118 @@
     <t>filelocation</t>
   </si>
   <si>
-    <t>/Volumes/Extreme/Projects/staging/data/1_Allison2_1_Embryo 1 end of nc12-gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/2_Allison2_2_Time course nc10 or 11 to gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/3_Allison2_3_nc 12 to gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/4_Allison2_4_Embryo 1 nc12-gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/5_Allison2_5_Embryo 2 nc11-gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/6_Etika_2021_04_06</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/7_Etika_2022_03_18</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/8_Sadia_1_embryo_1_nc10-gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/9_Sadia_2_embryo_1_nc10-gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/10_Sadia_3_embryo_1_nc12-gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/11_Sadia_4_embryo_1_nc10-nc14</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/12_Sadia_5_embryo_1_nc10-nc14</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/13_Sadia_6_embryo1-nc13-gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/14_Sadia_7_embryo2-nc11-nc14end</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/15_Sadia_8_embryo1-nc10-gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/16_Sadia_9_embryo1-nc10-gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/17_Sadia_10_embryo1-nc10-gastrulation</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/18_Images_2010-02-27_86H2A_xs_mdb_01timecourse</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/19_Images_2010-03-13_H2Arfp;dlgfp_xs_mdb_02timecourse</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/20_Images_2010-03-23_H2Arfp;dlgfp_xs_mdb_03timecourse</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/21_Images_2010-03-24_H2Arfp;dlgfp_xs_mdb_03timecourse</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/22_Images_2010-03-25_H2Arfp;dlgfp_xs_mdb_02timecourse</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/23_Images_2010-03-25_H2Arfp;dlgfp_xs_mdb_03timecourse</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/24_Images_2010-11-11_dl1dl4_86H2A_xs_mdb_02_timecourse</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/25_Images_2010-11-13_dl1CyO_86H2ATM3_xs_mdb_02_timecourse</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/26_Images_2010-12-20_dl1CyO_86H2ATM3_xs_mdb_01_timecourse</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/27_Images_2011-01-23_dlVenus-H2Arfp_live_mdb_embryo3_timecourse</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/28_Dosage_dorsal dosage good files_2018-01-30_2018-01-30 1 copy dorsal embryo 01</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/29_Dosage_dorsal dosage good files_2018-02-01_2018-02-01 2 copy dorsal embryo 01</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/30_Dosage_dorsal dosage good files_2018-02-02_2018-02-02 1 copy dorsal embryo 02</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/31_Dosage_dorsal dosage good files_2018-02-07_2018-02-07 1 copy dorsal</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/32_Dosage_dorsal dosage good files_2018-02-14_2018-02-14 4 copy dorsal embryo 03</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/33_Dosage_dorsal dosage good files_2018-02-24_2018-02-24 2 copy dorsal embryo 06</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/34_Dosage_dorsal dosage good files_2018-05-29_4 copy dorsal embryo 25</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/35_Dosage_dorsal dosage good files_2018-06-02_1 copy dorsal embryo 30</t>
-  </si>
-  <si>
-    <t>/Volumes/Extreme/Projects/staging/data/36_Dosage_dorsal dosage good files_2018-06-02_4 copy dorsal embryo 28</t>
+    <t>/Volumes/Extreme/Projects/staging/data/1_1_Embryo_1_end_of_nc12-gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/2_2_Time_course_nc10_or_11_to_gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/3_3_nc_12_to_gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/4_4_Embryo_1_nc12-gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/5_5_Embryo_2_nc11-gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/6_2021_04_06_lif</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/7_2022_03_18_lif</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/8_1_embryo_1_nc10-gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/9_2_embryo_1_nc10-gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/10_3_embryo_1_nc12-gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/11_4_embryo_1_nc10-nc14_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/12_5_embryo_1_nc10-nc14_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/13_6_embryo1-nc13-gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/14_7_embryo2-nc11-nc14end_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/15_8_embryo1-nc10-gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/16_9_embryo1-nc10-gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/17_10_embryo1-nc10-gastrulation_czi</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/18_2010-02-27_86H2A_xs_mdb_01timecourse_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/19_2010-03-13_H2Arfp_dlgfp_xs_mdb_02timecourse_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/20_2010-03-23_H2Arfp_dlgfp_xs_mdb_03timecourse_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/21_2010-03-24_H2Arfp_dlgfp_xs_mdb_03timecourse_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/22_2010-03-25_H2Arfp_dlgfp_xs_mdb_02timecourse_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/23_2010-03-25_H2Arfp_dlgfp_xs_mdb_03timecourse_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/24_2010-11-11_dl1dl4_86H2A_xs_mdb_02_timecourse_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/25_2010-11-13_dl1CyO_86H2ATM3_xs_mdb_02_timecourse_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/26_2010-12-20_dl1CyO_86H2ATM3_xs_mdb_01_timecourse_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/27_2011-01-23_dlVenus-H2Arfp_live_mdb_embryo3_timecourse_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/28_dorsal_dosage_good_files_2018-01-30_2018-01-30_1_copy_dorsal_embryo_01_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/29_dorsal_dosage_good_files_2018-02-01_2018-02-01_2_copy_dorsal_embryo_01_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/30_dorsal_dosage_good_files_2018-02-02_2018-02-02_1_copy_dorsal_embryo_02_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/31_dorsal_dosage_good_files_2018-02-07_2018-02-07_1_copy_dorsal_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/32_dorsal_dosage_good_files_2018-02-14_2018-02-14_4_copy_dorsal_embryo_03_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/33_dorsal_dosage_good_files_2018-02-24_2018-02-24_2_copy_dorsal_embryo_06_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/34_dorsal_dosage_good_files_2018-05-29_4_copy_dorsal_embryo_25_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/35_dorsal_dosage_good_files_2018-06-02_1_copy_dorsal_embryo_30_lsm</t>
+  </si>
+  <si>
+    <t>/Volumes/Extreme/Projects/staging/data/36_dorsal_dosage_good_files_2018-06-02_4_copy_dorsal_embryo_28_lsm</t>
+  </si>
+  <si>
+    <t>nc14start</t>
+  </si>
+  <si>
+    <t>nc14end</t>
   </si>
   <si>
     <t>sstart</t>
@@ -142,6 +148,21 @@
   </si>
   <si>
     <t>ch</t>
+  </si>
+  <si>
+    <t>filetype</t>
+  </si>
+  <si>
+    <t>czi</t>
+  </si>
+  <si>
+    <t>lif</t>
+  </si>
+  <si>
+    <t>czi</t>
+  </si>
+  <si>
+    <t>lsm</t>
   </si>
 </sst>
 </file>
@@ -187,16 +208,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:J37"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="true"/>
-    <col min="2" max="2" width="113" customWidth="true"/>
-    <col min="3" max="3" width="6" customWidth="true"/>
-    <col min="4" max="4" width="5.85546875" customWidth="true"/>
-    <col min="5" max="5" width="5.42578125" customWidth="true"/>
-    <col min="6" max="6" width="5.28515625" customWidth="true"/>
-    <col min="7" max="7" width="3.140625" customWidth="true"/>
+    <col min="2" max="2" width="114.28515625" customWidth="true"/>
+    <col min="3" max="3" width="9.140625" customWidth="true"/>
+    <col min="4" max="4" width="8.5703125" customWidth="true"/>
+    <col min="5" max="5" width="6" customWidth="true"/>
+    <col min="6" max="6" width="5.85546875" customWidth="true"/>
+    <col min="7" max="7" width="5.42578125" customWidth="true"/>
+    <col min="8" max="8" width="5.28515625" customWidth="true"/>
+    <col min="9" max="9" width="3.140625" customWidth="true"/>
+    <col min="10" max="10" width="8.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -221,6 +245,15 @@
       <c r="G1" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
@@ -230,19 +263,28 @@
         <v>2</v>
       </c>
       <c r="C2" s="0">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0">
+        <v>38</v>
+      </c>
+      <c r="E2" s="0">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0">
         <v>16</v>
       </c>
-      <c r="E2" s="0">
-        <v>1</v>
-      </c>
-      <c r="F2" s="0">
+      <c r="G2" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0">
         <v>38</v>
       </c>
-      <c r="G2" s="0">
-        <v>2</v>
+      <c r="I2" s="0">
+        <v>2</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -253,19 +295,28 @@
         <v>3</v>
       </c>
       <c r="C3" s="0">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D3" s="0">
+        <v>47</v>
+      </c>
+      <c r="E3" s="0">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0">
         <v>25</v>
       </c>
-      <c r="E3" s="0">
-        <v>1</v>
-      </c>
-      <c r="F3" s="0">
+      <c r="G3" s="0">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0">
         <v>47</v>
       </c>
-      <c r="G3" s="0">
-        <v>2</v>
+      <c r="I3" s="0">
+        <v>2</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4">
@@ -276,19 +327,28 @@
         <v>4</v>
       </c>
       <c r="C4" s="0">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0">
+        <v>48</v>
+      </c>
+      <c r="E4" s="0">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0">
         <v>20</v>
       </c>
-      <c r="E4" s="0">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0">
-        <v>48</v>
-      </c>
       <c r="G4" s="0">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="H4" s="0">
+        <v>48</v>
+      </c>
+      <c r="I4" s="0">
+        <v>2</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5">
@@ -299,19 +359,28 @@
         <v>5</v>
       </c>
       <c r="C5" s="0">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0">
+        <v>41</v>
+      </c>
+      <c r="E5" s="0">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0">
         <v>18</v>
       </c>
-      <c r="E5" s="0">
-        <v>1</v>
-      </c>
-      <c r="F5" s="0">
+      <c r="G5" s="0">
+        <v>1</v>
+      </c>
+      <c r="H5" s="0">
         <v>41</v>
       </c>
-      <c r="G5" s="0">
-        <v>2</v>
+      <c r="I5" s="0">
+        <v>2</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6">
@@ -322,19 +391,28 @@
         <v>6</v>
       </c>
       <c r="C6" s="0">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0">
+        <v>41</v>
+      </c>
+      <c r="E6" s="0">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0">
         <v>20</v>
       </c>
-      <c r="E6" s="0">
-        <v>1</v>
-      </c>
-      <c r="F6" s="0">
+      <c r="G6" s="0">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0">
         <v>41</v>
       </c>
-      <c r="G6" s="0">
-        <v>2</v>
+      <c r="I6" s="0">
+        <v>2</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7">
@@ -345,19 +423,28 @@
         <v>7</v>
       </c>
       <c r="C7" s="0">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="D7" s="0">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="E7" s="0">
         <v>5</v>
       </c>
       <c r="F7" s="0">
+        <v>64</v>
+      </c>
+      <c r="G7" s="0">
+        <v>5</v>
+      </c>
+      <c r="H7" s="0">
         <v>151</v>
       </c>
-      <c r="G7" s="0">
-        <v>1</v>
+      <c r="I7" s="0">
+        <v>1</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8">
@@ -368,19 +455,28 @@
         <v>8</v>
       </c>
       <c r="C8" s="0">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D8" s="0">
+        <v>129</v>
+      </c>
+      <c r="E8" s="0">
+        <v>2</v>
+      </c>
+      <c r="F8" s="0">
         <v>24</v>
       </c>
-      <c r="E8" s="0">
+      <c r="G8" s="0">
         <v>3</v>
       </c>
-      <c r="F8" s="0">
+      <c r="H8" s="0">
         <v>97</v>
       </c>
-      <c r="G8" s="0">
-        <v>1</v>
+      <c r="I8" s="0">
+        <v>1</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9">
@@ -391,19 +487,28 @@
         <v>9</v>
       </c>
       <c r="C9" s="0">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="D9" s="0">
+        <v>198</v>
+      </c>
+      <c r="E9" s="0">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0">
         <v>96</v>
       </c>
-      <c r="E9" s="0">
-        <v>1</v>
-      </c>
-      <c r="F9" s="0">
+      <c r="G9" s="0">
+        <v>1</v>
+      </c>
+      <c r="H9" s="0">
         <v>198</v>
       </c>
-      <c r="G9" s="0">
-        <v>2</v>
+      <c r="I9" s="0">
+        <v>2</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10">
@@ -414,19 +519,28 @@
         <v>10</v>
       </c>
       <c r="C10" s="0">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="D10" s="0">
+        <v>187</v>
+      </c>
+      <c r="E10" s="0">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0">
         <v>80</v>
       </c>
-      <c r="E10" s="0">
-        <v>1</v>
-      </c>
-      <c r="F10" s="0">
+      <c r="G10" s="0">
+        <v>1</v>
+      </c>
+      <c r="H10" s="0">
         <v>187</v>
       </c>
-      <c r="G10" s="0">
-        <v>2</v>
+      <c r="I10" s="0">
+        <v>2</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11">
@@ -437,19 +551,28 @@
         <v>11</v>
       </c>
       <c r="C11" s="0">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="D11" s="0">
+        <v>156</v>
+      </c>
+      <c r="E11" s="0">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0">
         <v>54</v>
       </c>
-      <c r="E11" s="0">
-        <v>1</v>
-      </c>
-      <c r="F11" s="0">
+      <c r="G11" s="0">
+        <v>1</v>
+      </c>
+      <c r="H11" s="0">
         <v>156</v>
       </c>
-      <c r="G11" s="0">
-        <v>2</v>
+      <c r="I11" s="0">
+        <v>2</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12">
@@ -460,19 +583,28 @@
         <v>12</v>
       </c>
       <c r="C12" s="0">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D12" s="0">
+        <v>188</v>
+      </c>
+      <c r="E12" s="0">
+        <v>1</v>
+      </c>
+      <c r="F12" s="0">
         <v>87</v>
       </c>
-      <c r="E12" s="0">
-        <v>1</v>
-      </c>
-      <c r="F12" s="0">
+      <c r="G12" s="0">
+        <v>1</v>
+      </c>
+      <c r="H12" s="0">
         <v>188</v>
       </c>
-      <c r="G12" s="0">
-        <v>2</v>
+      <c r="I12" s="0">
+        <v>2</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -483,19 +615,28 @@
         <v>13</v>
       </c>
       <c r="C13" s="0">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D13" s="0">
+        <v>196</v>
+      </c>
+      <c r="E13" s="0">
+        <v>1</v>
+      </c>
+      <c r="F13" s="0">
         <v>87</v>
       </c>
-      <c r="E13" s="0">
-        <v>1</v>
-      </c>
-      <c r="F13" s="0">
+      <c r="G13" s="0">
+        <v>1</v>
+      </c>
+      <c r="H13" s="0">
         <v>196</v>
       </c>
-      <c r="G13" s="0">
-        <v>2</v>
+      <c r="I13" s="0">
+        <v>2</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14">
@@ -506,19 +647,28 @@
         <v>14</v>
       </c>
       <c r="C14" s="0">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="D14" s="0">
+        <v>131</v>
+      </c>
+      <c r="E14" s="0">
+        <v>1</v>
+      </c>
+      <c r="F14" s="0">
         <v>39</v>
       </c>
-      <c r="E14" s="0">
-        <v>1</v>
-      </c>
-      <c r="F14" s="0">
+      <c r="G14" s="0">
+        <v>1</v>
+      </c>
+      <c r="H14" s="0">
         <v>131</v>
       </c>
-      <c r="G14" s="0">
-        <v>2</v>
+      <c r="I14" s="0">
+        <v>2</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15">
@@ -529,19 +679,28 @@
         <v>15</v>
       </c>
       <c r="C15" s="0">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="D15" s="0">
+        <v>170</v>
+      </c>
+      <c r="E15" s="0">
+        <v>1</v>
+      </c>
+      <c r="F15" s="0">
         <v>77</v>
       </c>
-      <c r="E15" s="0">
-        <v>1</v>
-      </c>
-      <c r="F15" s="0">
+      <c r="G15" s="0">
+        <v>1</v>
+      </c>
+      <c r="H15" s="0">
         <v>170</v>
       </c>
-      <c r="G15" s="0">
-        <v>2</v>
+      <c r="I15" s="0">
+        <v>2</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16">
@@ -552,19 +711,28 @@
         <v>16</v>
       </c>
       <c r="C16" s="0">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="D16" s="0">
+        <v>210</v>
+      </c>
+      <c r="E16" s="0">
+        <v>1</v>
+      </c>
+      <c r="F16" s="0">
         <v>108</v>
       </c>
-      <c r="E16" s="0">
-        <v>1</v>
-      </c>
-      <c r="F16" s="0">
+      <c r="G16" s="0">
+        <v>1</v>
+      </c>
+      <c r="H16" s="0">
         <v>210</v>
       </c>
-      <c r="G16" s="0">
-        <v>2</v>
+      <c r="I16" s="0">
+        <v>2</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17">
@@ -575,19 +743,28 @@
         <v>17</v>
       </c>
       <c r="C17" s="0">
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="D17" s="0">
+        <v>218</v>
+      </c>
+      <c r="E17" s="0">
+        <v>1</v>
+      </c>
+      <c r="F17" s="0">
         <v>119</v>
       </c>
-      <c r="E17" s="0">
-        <v>1</v>
-      </c>
-      <c r="F17" s="0">
+      <c r="G17" s="0">
+        <v>1</v>
+      </c>
+      <c r="H17" s="0">
         <v>218</v>
       </c>
-      <c r="G17" s="0">
-        <v>2</v>
+      <c r="I17" s="0">
+        <v>2</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18">
@@ -598,19 +775,28 @@
         <v>18</v>
       </c>
       <c r="C18" s="0">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D18" s="0">
+        <v>203</v>
+      </c>
+      <c r="E18" s="0">
+        <v>1</v>
+      </c>
+      <c r="F18" s="0">
         <v>102</v>
       </c>
-      <c r="E18" s="0">
-        <v>1</v>
-      </c>
-      <c r="F18" s="0">
+      <c r="G18" s="0">
+        <v>1</v>
+      </c>
+      <c r="H18" s="0">
         <v>203</v>
       </c>
-      <c r="G18" s="0">
-        <v>2</v>
+      <c r="I18" s="0">
+        <v>2</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19">
@@ -621,19 +807,28 @@
         <v>19</v>
       </c>
       <c r="C19" s="0">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D19" s="0">
+        <v>74</v>
+      </c>
+      <c r="E19" s="0">
+        <v>1</v>
+      </c>
+      <c r="F19" s="0">
         <v>42</v>
       </c>
-      <c r="E19" s="0">
-        <v>1</v>
-      </c>
-      <c r="F19" s="0">
+      <c r="G19" s="0">
+        <v>1</v>
+      </c>
+      <c r="H19" s="0">
         <v>74</v>
       </c>
-      <c r="G19" s="0">
-        <v>2</v>
+      <c r="I19" s="0">
+        <v>2</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20">
@@ -644,19 +839,28 @@
         <v>20</v>
       </c>
       <c r="C20" s="0">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D20" s="0">
+        <v>65</v>
+      </c>
+      <c r="E20" s="0">
+        <v>1</v>
+      </c>
+      <c r="F20" s="0">
         <v>32</v>
       </c>
-      <c r="E20" s="0">
-        <v>1</v>
-      </c>
-      <c r="F20" s="0">
+      <c r="G20" s="0">
+        <v>1</v>
+      </c>
+      <c r="H20" s="0">
         <v>65</v>
       </c>
-      <c r="G20" s="0">
-        <v>2</v>
+      <c r="I20" s="0">
+        <v>2</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21">
@@ -667,19 +871,28 @@
         <v>21</v>
       </c>
       <c r="C21" s="0">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="D21" s="0">
+        <v>170</v>
+      </c>
+      <c r="E21" s="0">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0">
         <v>65</v>
       </c>
-      <c r="E21" s="0">
-        <v>1</v>
-      </c>
-      <c r="F21" s="0">
+      <c r="G21" s="0">
+        <v>1</v>
+      </c>
+      <c r="H21" s="0">
         <v>170</v>
       </c>
-      <c r="G21" s="0">
-        <v>2</v>
+      <c r="I21" s="0">
+        <v>2</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22">
@@ -690,19 +903,28 @@
         <v>22</v>
       </c>
       <c r="C22" s="0">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D22" s="0">
-        <v>48</v>
+        <v>147</v>
       </c>
       <c r="E22" s="0">
         <v>1</v>
       </c>
       <c r="F22" s="0">
+        <v>48</v>
+      </c>
+      <c r="G22" s="0">
+        <v>1</v>
+      </c>
+      <c r="H22" s="0">
         <v>147</v>
       </c>
-      <c r="G22" s="0">
-        <v>2</v>
+      <c r="I22" s="0">
+        <v>2</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23">
@@ -713,19 +935,28 @@
         <v>23</v>
       </c>
       <c r="C23" s="0">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="D23" s="0">
+        <v>165</v>
+      </c>
+      <c r="E23" s="0">
+        <v>1</v>
+      </c>
+      <c r="F23" s="0">
         <v>55</v>
       </c>
-      <c r="E23" s="0">
-        <v>1</v>
-      </c>
-      <c r="F23" s="0">
+      <c r="G23" s="0">
+        <v>1</v>
+      </c>
+      <c r="H23" s="0">
         <v>165</v>
       </c>
-      <c r="G23" s="0">
-        <v>2</v>
+      <c r="I23" s="0">
+        <v>2</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24">
@@ -736,19 +967,28 @@
         <v>24</v>
       </c>
       <c r="C24" s="0">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="D24" s="0">
+        <v>156</v>
+      </c>
+      <c r="E24" s="0">
+        <v>1</v>
+      </c>
+      <c r="F24" s="0">
         <v>47</v>
       </c>
-      <c r="E24" s="0">
-        <v>1</v>
-      </c>
-      <c r="F24" s="0">
+      <c r="G24" s="0">
+        <v>1</v>
+      </c>
+      <c r="H24" s="0">
         <v>156</v>
       </c>
-      <c r="G24" s="0">
-        <v>2</v>
+      <c r="I24" s="0">
+        <v>2</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25">
@@ -759,19 +999,28 @@
         <v>25</v>
       </c>
       <c r="C25" s="0">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="D25" s="0">
+        <v>146</v>
+      </c>
+      <c r="E25" s="0">
+        <v>1</v>
+      </c>
+      <c r="F25" s="0">
         <v>64</v>
       </c>
-      <c r="E25" s="0">
-        <v>1</v>
-      </c>
-      <c r="F25" s="0">
+      <c r="G25" s="0">
+        <v>1</v>
+      </c>
+      <c r="H25" s="0">
         <v>146</v>
       </c>
-      <c r="G25" s="0">
-        <v>2</v>
+      <c r="I25" s="0">
+        <v>2</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="26">
@@ -782,19 +1031,28 @@
         <v>26</v>
       </c>
       <c r="C26" s="0">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D26" s="0">
+        <v>171</v>
+      </c>
+      <c r="E26" s="0">
+        <v>1</v>
+      </c>
+      <c r="F26" s="0">
         <v>103</v>
       </c>
-      <c r="E26" s="0">
-        <v>1</v>
-      </c>
-      <c r="F26" s="0">
+      <c r="G26" s="0">
+        <v>1</v>
+      </c>
+      <c r="H26" s="0">
         <v>171</v>
       </c>
-      <c r="G26" s="0">
-        <v>2</v>
+      <c r="I26" s="0">
+        <v>2</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27">
@@ -805,19 +1063,28 @@
         <v>27</v>
       </c>
       <c r="C27" s="0">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D27" s="0">
+        <v>72</v>
+      </c>
+      <c r="E27" s="0">
+        <v>1</v>
+      </c>
+      <c r="F27" s="0">
         <v>10</v>
       </c>
-      <c r="E27" s="0">
-        <v>1</v>
-      </c>
-      <c r="F27" s="0">
+      <c r="G27" s="0">
+        <v>1</v>
+      </c>
+      <c r="H27" s="0">
         <v>72</v>
       </c>
-      <c r="G27" s="0">
-        <v>2</v>
+      <c r="I27" s="0">
+        <v>2</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="28">
@@ -828,19 +1095,28 @@
         <v>28</v>
       </c>
       <c r="C28" s="0">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D28" s="0">
+        <v>42</v>
+      </c>
+      <c r="E28" s="0">
+        <v>1</v>
+      </c>
+      <c r="F28" s="0">
         <v>7</v>
       </c>
-      <c r="E28" s="0">
-        <v>1</v>
-      </c>
-      <c r="F28" s="0">
+      <c r="G28" s="0">
+        <v>1</v>
+      </c>
+      <c r="H28" s="0">
         <v>42</v>
       </c>
-      <c r="G28" s="0">
-        <v>1</v>
+      <c r="I28" s="0">
+        <v>1</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="29">
@@ -851,19 +1127,28 @@
         <v>29</v>
       </c>
       <c r="C29" s="0">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="D29" s="0">
+        <v>215</v>
+      </c>
+      <c r="E29" s="0">
+        <v>1</v>
+      </c>
+      <c r="F29" s="0">
         <v>126</v>
       </c>
-      <c r="E29" s="0">
-        <v>1</v>
-      </c>
-      <c r="F29" s="0">
+      <c r="G29" s="0">
+        <v>1</v>
+      </c>
+      <c r="H29" s="0">
         <v>215</v>
       </c>
-      <c r="G29" s="0">
-        <v>1</v>
+      <c r="I29" s="0">
+        <v>1</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="30">
@@ -874,19 +1159,28 @@
         <v>30</v>
       </c>
       <c r="C30" s="0">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="D30" s="0">
+        <v>175</v>
+      </c>
+      <c r="E30" s="0">
+        <v>1</v>
+      </c>
+      <c r="F30" s="0">
         <v>80</v>
       </c>
-      <c r="E30" s="0">
-        <v>1</v>
-      </c>
-      <c r="F30" s="0">
+      <c r="G30" s="0">
+        <v>1</v>
+      </c>
+      <c r="H30" s="0">
         <v>175</v>
       </c>
-      <c r="G30" s="0">
-        <v>1</v>
+      <c r="I30" s="0">
+        <v>1</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="31">
@@ -897,19 +1191,28 @@
         <v>31</v>
       </c>
       <c r="C31" s="0">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D31" s="0">
+        <v>164</v>
+      </c>
+      <c r="E31" s="0">
+        <v>1</v>
+      </c>
+      <c r="F31" s="0">
         <v>50</v>
       </c>
-      <c r="E31" s="0">
-        <v>1</v>
-      </c>
-      <c r="F31" s="0">
+      <c r="G31" s="0">
+        <v>1</v>
+      </c>
+      <c r="H31" s="0">
         <v>164</v>
       </c>
-      <c r="G31" s="0">
-        <v>1</v>
+      <c r="I31" s="0">
+        <v>1</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="32">
@@ -920,19 +1223,28 @@
         <v>32</v>
       </c>
       <c r="C32" s="0">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="D32" s="0">
+        <v>220</v>
+      </c>
+      <c r="E32" s="0">
+        <v>1</v>
+      </c>
+      <c r="F32" s="0">
         <v>97</v>
       </c>
-      <c r="E32" s="0">
-        <v>1</v>
-      </c>
-      <c r="F32" s="0">
+      <c r="G32" s="0">
+        <v>1</v>
+      </c>
+      <c r="H32" s="0">
         <v>220</v>
       </c>
-      <c r="G32" s="0">
-        <v>1</v>
+      <c r="I32" s="0">
+        <v>1</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="33">
@@ -943,19 +1255,28 @@
         <v>33</v>
       </c>
       <c r="C33" s="0">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D33" s="0">
+        <v>178</v>
+      </c>
+      <c r="E33" s="0">
+        <v>1</v>
+      </c>
+      <c r="F33" s="0">
         <v>79</v>
       </c>
-      <c r="E33" s="0">
-        <v>1</v>
-      </c>
-      <c r="F33" s="0">
+      <c r="G33" s="0">
+        <v>1</v>
+      </c>
+      <c r="H33" s="0">
         <v>178</v>
       </c>
-      <c r="G33" s="0">
-        <v>1</v>
+      <c r="I33" s="0">
+        <v>1</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="34">
@@ -966,19 +1287,28 @@
         <v>34</v>
       </c>
       <c r="C34" s="0">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D34" s="0">
+        <v>135</v>
+      </c>
+      <c r="E34" s="0">
+        <v>1</v>
+      </c>
+      <c r="F34" s="0">
         <v>24</v>
       </c>
-      <c r="E34" s="0">
-        <v>1</v>
-      </c>
-      <c r="F34" s="0">
+      <c r="G34" s="0">
+        <v>1</v>
+      </c>
+      <c r="H34" s="0">
         <v>135</v>
       </c>
-      <c r="G34" s="0">
-        <v>1</v>
+      <c r="I34" s="0">
+        <v>1</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="35">
@@ -989,19 +1319,28 @@
         <v>35</v>
       </c>
       <c r="C35" s="0">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D35" s="0">
+        <v>142</v>
+      </c>
+      <c r="E35" s="0">
+        <v>1</v>
+      </c>
+      <c r="F35" s="0">
         <v>32</v>
       </c>
-      <c r="E35" s="0">
-        <v>1</v>
-      </c>
-      <c r="F35" s="0">
+      <c r="G35" s="0">
+        <v>1</v>
+      </c>
+      <c r="H35" s="0">
         <v>142</v>
       </c>
-      <c r="G35" s="0">
-        <v>1</v>
+      <c r="I35" s="0">
+        <v>1</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="36">
@@ -1012,19 +1351,28 @@
         <v>36</v>
       </c>
       <c r="C36" s="0">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="D36" s="0">
+        <v>166</v>
+      </c>
+      <c r="E36" s="0">
+        <v>1</v>
+      </c>
+      <c r="F36" s="0">
         <v>55</v>
       </c>
-      <c r="E36" s="0">
-        <v>1</v>
-      </c>
-      <c r="F36" s="0">
+      <c r="G36" s="0">
+        <v>1</v>
+      </c>
+      <c r="H36" s="0">
         <v>166</v>
       </c>
-      <c r="G36" s="0">
-        <v>1</v>
+      <c r="I36" s="0">
+        <v>1</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="37">
@@ -1035,19 +1383,28 @@
         <v>37</v>
       </c>
       <c r="C37" s="0">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D37" s="0">
-        <v>48</v>
+        <v>164</v>
       </c>
       <c r="E37" s="0">
         <v>1</v>
       </c>
       <c r="F37" s="0">
+        <v>48</v>
+      </c>
+      <c r="G37" s="0">
+        <v>1</v>
+      </c>
+      <c r="H37" s="0">
         <v>164</v>
       </c>
-      <c r="G37" s="0">
-        <v>1</v>
+      <c r="I37" s="0">
+        <v>1</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>